<commit_message>
09.05.2023 Глумов v1.2 final
</commit_message>
<xml_diff>
--- a/Check-list.xlsx
+++ b/Check-list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Цель проекта</t>
   </si>
@@ -270,13 +270,16 @@
     <t>Есть наработки из предыдущей курсовой, можно их использовать</t>
   </si>
   <si>
-    <t>В базовом (бесплатном) курсе есть наработки, их также можно использовать</t>
-  </si>
-  <si>
     <t>Нужно проверить доступ</t>
   </si>
   <si>
     <t>Создано 4 таблицы</t>
+  </si>
+  <si>
+    <t>Выполнено</t>
+  </si>
+  <si>
+    <t>выполнено</t>
   </si>
 </sst>
 </file>
@@ -908,7 +911,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,6 +972,9 @@
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1075,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A28:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1116,7 @@
         <v>44</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>45</v>
@@ -1121,7 +1127,7 @@
         <v>33</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>47</v>
@@ -1132,56 +1138,65 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C33" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C40" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>40</v>
       </c>

</xml_diff>